<commit_message>
Updated template with 19 26 28 30 32 34 36 and 37 ft lenghs
</commit_message>
<xml_diff>
--- a/templates/CostingSheetTemplate.xlsx
+++ b/templates/CostingSheetTemplate.xlsx
@@ -13,20 +13,29 @@
   </bookViews>
   <sheets>
     <sheet name="L18.5" sheetId="1" r:id="rId1"/>
-    <sheet name="L20" sheetId="2" r:id="rId2"/>
-    <sheet name="L21" sheetId="3" r:id="rId3"/>
-    <sheet name="L22" sheetId="4" r:id="rId4"/>
-    <sheet name="L23" sheetId="5" r:id="rId5"/>
-    <sheet name="L24" sheetId="6" r:id="rId6"/>
-    <sheet name="L25" sheetId="7" r:id="rId7"/>
-    <sheet name="L27" sheetId="8" r:id="rId8"/>
-    <sheet name="L29" sheetId="9" r:id="rId9"/>
-    <sheet name="L31" sheetId="10" r:id="rId10"/>
-    <sheet name="L33" sheetId="11" r:id="rId11"/>
-    <sheet name="L35" sheetId="12" r:id="rId12"/>
+    <sheet name="L19" sheetId="14" r:id="rId2"/>
+    <sheet name="L20" sheetId="2" r:id="rId3"/>
+    <sheet name="L21" sheetId="3" r:id="rId4"/>
+    <sheet name="L22" sheetId="4" r:id="rId5"/>
+    <sheet name="L23" sheetId="5" r:id="rId6"/>
+    <sheet name="L24" sheetId="6" r:id="rId7"/>
+    <sheet name="L25" sheetId="7" r:id="rId8"/>
+    <sheet name="L26" sheetId="15" r:id="rId9"/>
+    <sheet name="L27" sheetId="8" r:id="rId10"/>
+    <sheet name="L28" sheetId="16" r:id="rId11"/>
+    <sheet name="L29" sheetId="9" r:id="rId12"/>
+    <sheet name="L30" sheetId="17" r:id="rId13"/>
+    <sheet name="L31" sheetId="10" r:id="rId14"/>
+    <sheet name="L32" sheetId="18" r:id="rId15"/>
+    <sheet name="L33" sheetId="11" r:id="rId16"/>
+    <sheet name="L34" sheetId="19" r:id="rId17"/>
+    <sheet name="L35" sheetId="12" r:id="rId18"/>
+    <sheet name="L36" sheetId="20" r:id="rId19"/>
+    <sheet name="L37" sheetId="21" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'L18.5'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'L19'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="9">
   <si>
     <t>Vendor</t>
   </si>
@@ -445,7 +454,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -551,68 +560,468 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" customWidth="1"/>
-    <col min="6" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -673,6 +1082,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="80" orientation="landscape" horizontalDpi="4294967293"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -731,64 +1198,64 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32:B34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" customWidth="1"/>
-    <col min="6" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>